<commit_message>
editar visita desde rutear
</commit_message>
<xml_diff>
--- a/src/assets/ejemplos/modelo/estructuraVisita.xlsx
+++ b/src/assets/ejemplos/modelo/estructuraVisita.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">guia</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t xml:space="preserve">numero</t>
   </si>
   <si>
     <t xml:space="preserve">fecha</t>
@@ -61,10 +61,13 @@
     <t xml:space="preserve">decodificado</t>
   </si>
   <si>
+    <t xml:space="preserve">tiempo_servicio</t>
+  </si>
+  <si>
     <t xml:space="preserve">MARCO SANCHEZ</t>
   </si>
   <si>
-    <t xml:space="preserve">CR 40 65AA - 22 B. Villa Hermosa</t>
+    <t xml:space="preserve">CR 40 65AA - 22 B. Villa Hermosa, MEDELLIN</t>
   </si>
 </sst>
 </file>
@@ -97,12 +100,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6D6D"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -139,12 +148,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -157,94 +174,274 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF6D6D"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>20241001</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>11111</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>3201457478</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="I2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat: Ajustes generar ciclo de revision alexander martinez 2025-09-09
</commit_message>
<xml_diff>
--- a/src/assets/ejemplos/modelo/estructuraVisita.xlsx
+++ b/src/assets/ejemplos/modelo/estructuraVisita.xlsx
@@ -37,13 +37,13 @@
     <t xml:space="preserve">destinatario_direccion</t>
   </si>
   <si>
-    <t xml:space="preserve">ciudad</t>
-  </si>
-  <si>
     <t xml:space="preserve">destinatario_telefono</t>
   </si>
   <si>
     <t xml:space="preserve">destinatario_correo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unidades</t>
   </si>
   <si>
     <t xml:space="preserve">peso</t>
@@ -351,17 +351,16 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.39"/>
   </cols>
   <sheetData>
@@ -426,10 +425,10 @@
         <v>15</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="n">
         <v>3201457478</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="I2" s="2" t="n">
         <v>1</v>
@@ -449,8 +448,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>